<commit_message>
Add vercel URL for cors
</commit_message>
<xml_diff>
--- a/backened/public/audit-reports.xlsx
+++ b/backened/public/audit-reports.xlsx
@@ -73,10 +73,52 @@
     <t>0.00</t>
   </si>
   <si>
-    <t>23/11/2025</t>
-  </si>
-  <si>
-    <t>{"FO1":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"FO2":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"FO3":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":"hello kais ho aap"},"FO4":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"FO5":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP1":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP2":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP3":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP4":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP5":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP6":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP7":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP8":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP9":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP10":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"PP1":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"PP2":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"MP1":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"MP2":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"MP3":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"MP4":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"MP5":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""}}</t>
+    <t>25/11/2025</t>
+  </si>
+  <si>
+    <t>{"FO1":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"FO2":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"FO3":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"FO4":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"FO5":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP1":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP2":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP3":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP4":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP5":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP6":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP7":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP8":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP9":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP10":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"PP1":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"PP2":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"MP1":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"MP2":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"MP3":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"MP4":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"MP5":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""}}</t>
+  </si>
+  <si>
+    <t>Not Submitted</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>CC002</t>
+  </si>
+  <si>
+    <t>NIIT Mumbai</t>
+  </si>
+  <si>
+    <t>Mumbai Br.</t>
+  </si>
+  <si>
+    <t>19.0760° N,72.8777°</t>
+  </si>
+  <si>
+    <t>Priya Singh</t>
+  </si>
+  <si>
+    <t>Suresh Patel</t>
+  </si>
+  <si>
+    <t>29.40</t>
+  </si>
+  <si>
+    <t>26.00</t>
+  </si>
+  <si>
+    <t>15.00</t>
+  </si>
+  <si>
+    <t>85.40</t>
+  </si>
+  <si>
+    <t>19/11/2025</t>
+  </si>
+  <si>
+    <t>{"FO1":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":9,"remarks":"50"},"FO2":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":6,"remarks":"50"},"FO3":{"totalSamples":"50","samplesCompliant":"14","compliantPercent":28,"score":0,"remarks":"05"},"FO4":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":12,"remarks":"50"},"FO5":{"totalSamples":"50","samplesCompliant":"40","compliantPercent":80,"score":2.4,"remarks":""},"DP1":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":6,"remarks":"50"},"DP2":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":4,"remarks":"50"},"DP3":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":6,"remarks":"50"},"DP4":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":2,"remarks":"50"},"DP5":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":4,"remarks":"50"},"DP6":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":4,"remarks":"50"},"DP7":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP8":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP9":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP10":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"PP1":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":4.5,"remarks":"0"},"PP2":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":10.5,"remarks":"05"},"MP1":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":0.75,"remarks":"50"},"MP2":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":3.75,"remarks":"50"},"MP3":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":5.25,"remarks":"50"},"MP4":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":4.5,"remarks":"50"},"MP5":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":0.75,"remarks":"50"}}</t>
   </si>
   <si>
     <t>Submitted</t>
@@ -86,48 +128,6 @@
   </si>
   <si>
     <t>Admin User</t>
-  </si>
-  <si>
-    <t>23/11/2025, 12:48:21</t>
-  </si>
-  <si>
-    <t>hi</t>
-  </si>
-  <si>
-    <t>CC002</t>
-  </si>
-  <si>
-    <t>NIIT Mumbai</t>
-  </si>
-  <si>
-    <t>Mumbai Br.</t>
-  </si>
-  <si>
-    <t>19.0760° N,72.8777°</t>
-  </si>
-  <si>
-    <t>Priya Singh</t>
-  </si>
-  <si>
-    <t>Suresh Patel</t>
-  </si>
-  <si>
-    <t>29.40</t>
-  </si>
-  <si>
-    <t>26.00</t>
-  </si>
-  <si>
-    <t>15.00</t>
-  </si>
-  <si>
-    <t>85.40</t>
-  </si>
-  <si>
-    <t>19/11/2025</t>
-  </si>
-  <si>
-    <t>{"FO1":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":9,"remarks":"50"},"FO2":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":6,"remarks":"50"},"FO3":{"totalSamples":"50","samplesCompliant":"14","compliantPercent":28,"score":0,"remarks":"05"},"FO4":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":12,"remarks":"50"},"FO5":{"totalSamples":"50","samplesCompliant":"40","compliantPercent":80,"score":2.4,"remarks":""},"DP1":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":6,"remarks":"50"},"DP2":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":4,"remarks":"50"},"DP3":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":6,"remarks":"50"},"DP4":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":2,"remarks":"50"},"DP5":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":4,"remarks":"50"},"DP6":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":4,"remarks":"50"},"DP7":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP8":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP9":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"DP10":{"totalSamples":"","samplesCompliant":"","compliantPercent":0,"score":0,"remarks":""},"PP1":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":4.5,"remarks":"0"},"PP2":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":10.5,"remarks":"05"},"MP1":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":0.75,"remarks":"50"},"MP2":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":3.75,"remarks":"50"},"MP3":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":5.25,"remarks":"50"},"MP4":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":4.5,"remarks":"50"},"MP5":{"totalSamples":"50","samplesCompliant":"50","compliantPercent":100,"score":0.75,"remarks":"50"}}</t>
   </si>
   <si>
     <t>20/11/2025, 09:42:03</t>
@@ -645,66 +645,66 @@
         <v>22</v>
       </c>
       <c r="O2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
       <c r="Q2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
         <v>33</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>34</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>35</v>
       </c>
-      <c r="J3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>36</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
         <v>37</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>38</v>
-      </c>
-      <c r="N3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" t="s">
-        <v>24</v>
       </c>
       <c r="Q3" t="s">
         <v>39</v>
@@ -754,13 +754,13 @@
         <v>48</v>
       </c>
       <c r="N4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="O4" t="s">
         <v>49</v>
       </c>
       <c r="P4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="Q4" t="s">
         <v>50</v>

</xml_diff>